<commit_message>
added some more informationen for the lysosome protocol
</commit_message>
<xml_diff>
--- a/optobiology.xlsx
+++ b/optobiology.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janpiotraschke/git_repos/fachkurs_optobiology/analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janpiotraschke/git_repos/fachkurs_optobiology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A676DCB5-1793-014E-A359-CA96B9AB0B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB6079A-986D-6748-BFDD-D0740E6E9D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{0747FCF5-9BB9-A240-971F-88470ED95DB6}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="2a-Lysosomes" sheetId="3" r:id="rId3"/>
     <sheet name="2b-EB3 comets" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="150">
   <si>
     <t>-</t>
   </si>
@@ -576,9 +576,6 @@
     <t>Student 2</t>
   </si>
   <si>
-    <t>DMEM</t>
-  </si>
-  <si>
     <t>Fugene</t>
   </si>
   <si>
@@ -601,12 +598,6 @@
     </r>
   </si>
   <si>
-    <t>delute the DNA with the 10x H2O volume</t>
-  </si>
-  <si>
-    <t>first add the DMEM</t>
-  </si>
-  <si>
     <t>then add the fugene and mix carefully</t>
   </si>
   <si>
@@ -641,6 +632,21 @@
   </si>
   <si>
     <t>add 200uL of each transfection mix dropwise to a well</t>
+  </si>
+  <si>
+    <t>DMEM-</t>
+  </si>
+  <si>
+    <t>first add the DMEM-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fugene </t>
+  </si>
+  <si>
+    <t>lamp1 DNA  [0.1ug/uL]</t>
+  </si>
+  <si>
+    <t>delute the 1ug/uL DNA with the 10x H2O volume to 0.1ug/uL</t>
   </si>
 </sst>
 </file>
@@ -648,7 +654,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -988,9 +994,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1002,51 +1005,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1104,7 +1080,37 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1429,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32C55F2-64D1-5747-8AFC-58CEA49DB674}">
   <dimension ref="A1:R126"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="I5:Q11"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,221 +1451,221 @@
         <v>44739</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="25" t="s">
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="25" t="s">
+      <c r="N5" s="57"/>
+      <c r="O5" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="P5" s="26" t="s">
+      <c r="P5" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="Q5" s="19" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="21" t="s">
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="N6" s="55"/>
+      <c r="O6" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="18" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="28" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="29" t="s">
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="28"/>
-      <c r="O7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="30" t="s">
+      <c r="N7" s="58"/>
+      <c r="O7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="Q7" s="29" t="s">
+      <c r="Q7" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="21" t="s">
+      <c r="J8" s="55"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="21" t="s">
+      <c r="N8" s="55"/>
+      <c r="O8" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="18" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="29" t="s">
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="N9" s="28"/>
-      <c r="O9" s="29" t="s">
+      <c r="N9" s="58"/>
+      <c r="O9" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="30" t="s">
+      <c r="P9" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="Q9" s="29" t="s">
+      <c r="Q9" s="21" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="13" t="s">
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="N10" s="13"/>
-      <c r="O10" s="21" t="s">
+      <c r="N10" s="55"/>
+      <c r="O10" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="12">
         <v>65906</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="Q10" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="R10" s="55" t="s">
+      <c r="R10" s="45" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" s="32" t="s">
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="N11" s="32"/>
-      <c r="O11" s="33" t="s">
+      <c r="N11" s="53"/>
+      <c r="O11" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="33"/>
-    </row>
-    <row r="13" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="P11" s="24"/>
+      <c r="Q11" s="23"/>
+    </row>
+    <row r="13" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1703,57 +1709,57 @@
     <row r="21" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="C21" s="1"/>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="6" t="s">
+      <c r="F21" s="55"/>
+      <c r="G21" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="J21" s="12"/>
+      <c r="H21" s="59"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F22" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="14"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="15"/>
+      <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="57" t="s">
+      <c r="F23" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="16"/>
+      <c r="G23" s="14"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="15"/>
+      <c r="I23" s="13"/>
     </row>
     <row r="24" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="C24" s="1"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="16"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="14"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="18"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K25" t="s">
@@ -1774,10 +1780,10 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H30" s="48" t="s">
+      <c r="H30" s="38" t="s">
         <v>2</v>
       </c>
       <c r="M30" t="s">
@@ -1792,7 +1798,7 @@
       <c r="D31">
         <v>100</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>101</v>
       </c>
       <c r="G31" t="s">
@@ -1804,27 +1810,27 @@
       <c r="I31" t="s">
         <v>103</v>
       </c>
-      <c r="K31" s="18" t="s">
+      <c r="K31" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="L31" s="18"/>
-      <c r="M31" s="53" t="s">
+      <c r="L31" s="16"/>
+      <c r="M31" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="10">
         <v>1</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="39" t="s">
         <v>101</v>
       </c>
       <c r="G32" t="s">
@@ -1836,16 +1842,16 @@
       <c r="I32" t="s">
         <v>103</v>
       </c>
-      <c r="K32" s="52" t="s">
+      <c r="K32" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="L32" s="43"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
@@ -1862,120 +1868,120 @@
         <f>H31/H32</f>
         <v>400</v>
       </c>
-      <c r="K33" s="52" t="s">
+      <c r="K33" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18" t="s">
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="O33" s="18"/>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="K34" s="42"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18" t="s">
+      <c r="K34" s="32"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="O34" s="18"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C35" s="45" t="s">
+      <c r="C35" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="45">
+      <c r="D35" s="35">
         <f>D37/D33</f>
         <v>30</v>
       </c>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G35" s="46" t="s">
+      <c r="G35" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H35" s="46">
+      <c r="H35" s="36">
         <f>H37/H33</f>
         <v>7.5</v>
       </c>
-      <c r="I35" s="46" t="s">
+      <c r="I35" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="K35" s="42"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="54" t="s">
+      <c r="K35" s="32"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="O35" s="18"/>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="45">
+      <c r="D36" s="35">
         <f>D37-D35</f>
         <v>2970</v>
       </c>
-      <c r="E36" s="45" t="s">
+      <c r="E36" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="51" t="s">
+      <c r="G36" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="46">
+      <c r="H36" s="36">
         <f>H37-H35</f>
         <v>2992.5</v>
       </c>
-      <c r="I36" s="46" t="s">
+      <c r="I36" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="K36" s="42"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="42"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="45">
+      <c r="D37" s="35">
         <v>3000</v>
       </c>
-      <c r="E37" s="45" t="s">
+      <c r="E37" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="46" t="s">
+      <c r="G37" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="46">
+      <c r="H37" s="36">
         <v>3000</v>
       </c>
-      <c r="I37" s="46" t="s">
+      <c r="I37" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="K37" s="42"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="42"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
@@ -2001,9 +2007,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
-      <c r="B45" s="8" t="s">
+    <row r="45" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2065,7 +2071,7 @@
       <c r="D57">
         <v>20</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2076,7 +2082,7 @@
       <c r="D58">
         <v>0.2</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2093,41 +2099,41 @@
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="8">
         <f>D63/D59</f>
         <v>12.5</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E61" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="8">
         <f>D63-D61</f>
         <v>1237.5</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E62" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C63" s="35" t="s">
+      <c r="C63" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D63" s="7">
         <f>D55*D56</f>
         <v>1250</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E63" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="10" t="s">
+      <c r="F63" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2196,41 +2202,41 @@
       <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D80" s="9">
+      <c r="D80" s="8">
         <f>D83/D77</f>
         <v>1.5</v>
       </c>
-      <c r="E80" s="9" t="s">
+      <c r="E80" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C81" s="7" t="s">
+      <c r="C81" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D81" s="9">
+      <c r="D81" s="8">
         <f>D83/D78</f>
         <v>1</v>
       </c>
-      <c r="E81" s="9" t="s">
+      <c r="E81" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D82" s="9">
+      <c r="D82" s="8">
         <f>D83</f>
         <v>600</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="E82" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F82" s="10" t="s">
+      <c r="F82" s="9" t="s">
         <v>53</v>
       </c>
       <c r="M82" t="s">
@@ -2238,16 +2244,16 @@
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C83" s="35" t="s">
+      <c r="C83" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="8">
+      <c r="D83" s="7">
         <v>600</v>
       </c>
-      <c r="E83" s="9" t="s">
+      <c r="E83" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="F83" s="9" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2315,50 +2321,50 @@
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C101" s="7" t="s">
+      <c r="C101" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D101" s="8">
         <f>D105/D97</f>
         <v>0.5</v>
       </c>
-      <c r="E101" s="9" t="s">
+      <c r="E101" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C102" s="7" t="s">
+      <c r="C102" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D102" s="9">
+      <c r="D102" s="8">
         <f>D105/D98</f>
         <v>0.5</v>
       </c>
-      <c r="E102" s="9" t="s">
+      <c r="E102" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C103" s="7" t="s">
+      <c r="C103" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D103" s="9">
+      <c r="D103" s="8">
         <f>D105/D99</f>
         <v>2</v>
       </c>
-      <c r="E103" s="9" t="s">
+      <c r="E103" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C104" s="7" t="s">
+      <c r="C104" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D104" s="8">
         <f>D105</f>
         <v>200</v>
       </c>
-      <c r="E104" s="9" t="s">
+      <c r="E104" s="8" t="s">
         <v>35</v>
       </c>
       <c r="M104" t="s">
@@ -2366,16 +2372,16 @@
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C105" s="35" t="s">
+      <c r="C105" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D105" s="8">
+      <c r="D105" s="7">
         <v>200</v>
       </c>
-      <c r="E105" s="9" t="s">
+      <c r="E105" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F105" s="10" t="s">
+      <c r="F105" s="9" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2440,41 +2446,41 @@
       <c r="C116" s="1"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C117" s="7" t="s">
+      <c r="C117" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D117" s="9">
+      <c r="D117" s="8">
         <f>D119/D115</f>
         <v>0.5</v>
       </c>
-      <c r="E117" s="9" t="s">
+      <c r="E117" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C118" s="7" t="s">
+      <c r="C118" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D118" s="9">
+      <c r="D118" s="8">
         <f>D119</f>
         <v>500</v>
       </c>
-      <c r="E118" s="9" t="s">
+      <c r="E118" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D119" s="9">
+      <c r="D119" s="8">
         <f>100*H113</f>
         <v>500</v>
       </c>
-      <c r="E119" s="9" t="s">
+      <c r="E119" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F119" s="10" t="s">
+      <c r="F119" s="9" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2487,28 +2493,28 @@
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A123" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B123" s="11" t="s">
+      <c r="A123" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="11"/>
-      <c r="G123" s="11"/>
-      <c r="H123" s="11"/>
-      <c r="I123" s="37"/>
-      <c r="J123" s="37"/>
-      <c r="K123" s="37"/>
-      <c r="L123" s="37"/>
-      <c r="M123" s="37"/>
-      <c r="N123" s="37"/>
-      <c r="O123" s="37"/>
-      <c r="P123" s="37"/>
-      <c r="Q123" s="37"/>
-      <c r="R123" s="37"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="27"/>
+      <c r="J123" s="27"/>
+      <c r="K123" s="27"/>
+      <c r="L123" s="27"/>
+      <c r="M123" s="27"/>
+      <c r="N123" s="27"/>
+      <c r="O123" s="27"/>
+      <c r="P123" s="27"/>
+      <c r="Q123" s="27"/>
+      <c r="R123" s="27"/>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
@@ -2528,6 +2534,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="M5:N5"/>
@@ -2536,14 +2550,6 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2563,28 +2569,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="17"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="17"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
@@ -2598,15 +2604,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B418F536-D2A8-4F42-BEB3-EBF867EDFB00}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2618,9 +2626,9 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2629,7 +2637,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
@@ -2638,7 +2646,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
@@ -2647,7 +2655,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="28" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
@@ -2656,7 +2664,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
@@ -2665,7 +2673,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
@@ -2674,7 +2682,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
@@ -2687,10 +2695,10 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
-        <v>139</v>
+    <row r="13" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2701,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2712,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2720,14 +2728,14 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="C19" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>132</v>
+      <c r="C19" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2735,14 +2743,14 @@
       <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="62">
+      <c r="C20" s="52">
         <f>2*200</f>
         <v>400</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="52">
         <v>9.6</v>
       </c>
-      <c r="E20" s="62">
+      <c r="E20" s="52">
         <v>32</v>
       </c>
     </row>
@@ -2775,110 +2783,110 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" s="1"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="58"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="48"/>
     </row>
     <row r="27" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="58"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="48"/>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8" t="s">
-        <v>144</v>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D34" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F34" s="9" t="s">
+      <c r="E34" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="F34" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="H34" s="9" t="s">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E35" t="s">
+      <c r="D35" s="52">
+        <v>200</v>
+      </c>
+      <c r="E35" s="52">
+        <v>4.8</v>
+      </c>
+      <c r="F35" s="52">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
         <v>133</v>
       </c>
-      <c r="F35" s="62">
-        <v>200</v>
-      </c>
-      <c r="G35" s="62">
-        <v>4.8</v>
-      </c>
-      <c r="H35" s="62">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" t="s">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2886,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2894,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some comments for the Lysosome protocol
</commit_message>
<xml_diff>
--- a/optobiology.xlsx
+++ b/optobiology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janpiotraschke/git_repos/fachkurs_optobiology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB6079A-986D-6748-BFDD-D0740E6E9D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C2DB0-5EB3-294C-BAE7-F0AD23A4A90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{0747FCF5-9BB9-A240-971F-88470ED95DB6}"/>
   </bookViews>
@@ -598,24 +598,15 @@
     </r>
   </si>
   <si>
-    <t>then add the fugene and mix carefully</t>
-  </si>
-  <si>
     <t>incubate for 5min</t>
   </si>
   <si>
-    <t xml:space="preserve">add the DNA and mix </t>
-  </si>
-  <si>
     <t>Preparation</t>
   </si>
   <si>
     <t xml:space="preserve">incubate for 15-20min at room temperature </t>
   </si>
   <si>
-    <t xml:space="preserve">repeat the transfection protocoll for the other well </t>
-  </si>
-  <si>
     <t>preheat 15ml growing Medium in the water bath to 37°C</t>
   </si>
   <si>
@@ -625,15 +616,9 @@
     <t xml:space="preserve">Transfection Protocol </t>
   </si>
   <si>
-    <t>Prepare the transfection mix in an Epi:</t>
-  </si>
-  <si>
     <t>incubate</t>
   </si>
   <si>
-    <t>add 200uL of each transfection mix dropwise to a well</t>
-  </si>
-  <si>
     <t>DMEM-</t>
   </si>
   <si>
@@ -646,7 +631,124 @@
     <t>lamp1 DNA  [0.1ug/uL]</t>
   </si>
   <si>
-    <t>delute the 1ug/uL DNA with the 10x H2O volume to 0.1ug/uL</t>
+    <t>repeat the transfection protocoll for the other Eppi</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">delute the 1ug/uL DNA with the 10x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>H2O (Dnase/Rnase free Water or VE-Water)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> volume to 0.1ug/uL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">then add the fugene and mix </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>how to mix?)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> carefully</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">add the DNA and mix </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>(how?)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prepare the transfection mix in an Eppi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>(or can we do it all in ones?)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">add 200uL of each transfection mix dropwise </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t xml:space="preserve">(also nicht an der Wand runterlaufen lassen !) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to a well</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -656,7 +758,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -694,6 +796,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri (Textkörper)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri (Textkörper)"/>
     </font>
   </fonts>
@@ -1081,34 +1189,34 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1435,7 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32C55F2-64D1-5747-8AFC-58CEA49DB674}">
   <dimension ref="A1:R126"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="D31" sqref="D31:D32"/>
     </sheetView>
   </sheetViews>
@@ -1468,18 +1576,18 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
       <c r="L5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="57" t="s">
+      <c r="M5" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="57"/>
+      <c r="N5" s="56"/>
       <c r="O5" s="19" t="s">
         <v>86</v>
       </c>
@@ -1497,18 +1605,18 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
       <c r="L6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="55" t="s">
+      <c r="M6" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="N6" s="55"/>
+      <c r="N6" s="53"/>
       <c r="O6" s="18" t="s">
         <v>0</v>
       </c>
@@ -1526,18 +1634,18 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
       <c r="L7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="58" t="s">
+      <c r="M7" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="58"/>
+      <c r="N7" s="59"/>
       <c r="O7" s="21" t="s">
         <v>0</v>
       </c>
@@ -1558,18 +1666,18 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="62"/>
       <c r="L8" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="M8" s="55" t="s">
+      <c r="M8" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="N8" s="55"/>
+      <c r="N8" s="53"/>
       <c r="O8" s="18" t="s">
         <v>81</v>
       </c>
@@ -1587,18 +1695,18 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="61" t="s">
+      <c r="I9" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
       <c r="L9" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="58" t="s">
+      <c r="M9" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="N9" s="58"/>
+      <c r="N9" s="59"/>
       <c r="O9" s="21" t="s">
         <v>82</v>
       </c>
@@ -1616,18 +1724,18 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
       <c r="L10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="55" t="s">
+      <c r="M10" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="N10" s="55"/>
+      <c r="N10" s="53"/>
       <c r="O10" s="18" t="s">
         <v>83</v>
       </c>
@@ -1642,18 +1750,18 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I11" s="62" t="s">
+      <c r="I11" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
       <c r="L11" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="M11" s="53" t="s">
+      <c r="M11" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="N11" s="53"/>
+      <c r="N11" s="61"/>
       <c r="O11" s="23" t="s">
         <v>84</v>
       </c>
@@ -1709,14 +1817,14 @@
     <row r="21" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="C21" s="1"/>
-      <c r="E21" s="55" t="s">
+      <c r="E21" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="55"/>
-      <c r="G21" s="59" t="s">
+      <c r="F21" s="53"/>
+      <c r="G21" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="59"/>
+      <c r="H21" s="54"/>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2534,6 +2642,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="I5:K5"/>
@@ -2542,14 +2658,6 @@
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I11:K11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2604,10 +2712,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B418F536-D2A8-4F42-BEB3-EBF867EDFB00}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2698,7 +2806,7 @@
     <row r="13" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2709,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2720,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2728,125 +2836,107 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="C19" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="48"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="48"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="52">
+      <c r="C31" s="52">
         <f>2*200</f>
         <v>400</v>
       </c>
-      <c r="D20" s="52">
+      <c r="D31" s="52">
         <v>9.6</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E31" s="52">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-      <c r="D25" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" t="s">
-        <v>128</v>
-      </c>
-      <c r="F25" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C26" s="1"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="48"/>
-    </row>
-    <row r="27" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="48"/>
-    </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="3"/>
-    </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D34" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E34" s="8" t="s">
+      <c r="B34" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D36" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>132</v>
       </c>
-      <c r="D35" s="52">
+      <c r="D37" s="52">
         <v>200</v>
       </c>
-      <c r="E35" s="52">
+      <c r="E37" s="52">
         <v>4.8</v>
       </c>
-      <c r="F35" s="52">
+      <c r="F37" s="52">
         <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2854,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2862,7 +2952,15 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2870,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2878,15 +2976,15 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2894,7 +2992,7 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2902,7 +3000,15 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected excel protocol 1b
</commit_message>
<xml_diff>
--- a/optobiology.xlsx
+++ b/optobiology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janpiotraschke/git_repos/fachkurs_optobiology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F591D356-A802-4245-A367-EF8FA81FAC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62041387-3C04-7742-96B7-19F53143E366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="1" xr2:uid="{0747FCF5-9BB9-A240-971F-88470ED95DB6}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="186">
   <si>
     <t>-</t>
   </si>
@@ -750,9 +750,6 @@
     </r>
   </si>
   <si>
-    <t>mouse anti-acetyl-tubulin</t>
-  </si>
-  <si>
     <t>sc-23950</t>
   </si>
   <si>
@@ -1159,6 +1156,21 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Phalloidin-Atto-488</t>
+  </si>
+  <si>
+    <t>1° - mouse anti-acetyl-tubulin</t>
+  </si>
+  <si>
+    <t>2° - anti mouse Alexa Fluor 568</t>
+  </si>
+  <si>
+    <t>2° - anti tubulin- Alexa Fluor 647</t>
+  </si>
+  <si>
+    <t>A-11031</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1213,13 +1225,6 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Textkörper)"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1514,7 +1519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1632,31 +1637,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1668,14 +1688,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2001,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32C55F2-64D1-5747-8AFC-58CEA49DB674}">
   <dimension ref="A1:R126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2034,18 +2057,18 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="62" t="s">
+      <c r="I5" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
       <c r="L5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="63"/>
+      <c r="N5" s="69"/>
       <c r="O5" s="18" t="s">
         <v>85</v>
       </c>
@@ -2063,18 +2086,18 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
       <c r="L6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="60" t="s">
+      <c r="M6" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="60"/>
+      <c r="N6" s="67"/>
       <c r="O6" s="17" t="s">
         <v>0</v>
       </c>
@@ -2092,18 +2115,18 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="65" t="s">
+      <c r="I7" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
       <c r="L7" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="66" t="s">
+      <c r="M7" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="66"/>
+      <c r="N7" s="70"/>
       <c r="O7" s="20" t="s">
         <v>0</v>
       </c>
@@ -2124,18 +2147,18 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="60"/>
-      <c r="K8" s="69"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
       <c r="L8" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="M8" s="60" t="s">
+      <c r="M8" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="N8" s="60"/>
+      <c r="N8" s="67"/>
       <c r="O8" s="17" t="s">
         <v>80</v>
       </c>
@@ -2153,18 +2176,18 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="65" t="s">
+      <c r="I9" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
       <c r="L9" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="M9" s="66" t="s">
+      <c r="M9" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="66"/>
+      <c r="N9" s="70"/>
       <c r="O9" s="20" t="s">
         <v>81</v>
       </c>
@@ -2182,18 +2205,18 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="64" t="s">
+      <c r="I10" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
       <c r="L10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="60" t="s">
+      <c r="M10" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="N10" s="60"/>
+      <c r="N10" s="67"/>
       <c r="O10" s="17" t="s">
         <v>82</v>
       </c>
@@ -2208,18 +2231,18 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="M11" s="68" t="s">
+      <c r="M11" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="N11" s="68"/>
+      <c r="N11" s="65"/>
       <c r="O11" s="22" t="s">
         <v>83</v>
       </c>
@@ -2275,14 +2298,14 @@
     <row r="21" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="C21" s="1"/>
-      <c r="E21" s="60" t="s">
+      <c r="E21" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61" t="s">
+      <c r="F21" s="67"/>
+      <c r="G21" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="61"/>
+      <c r="H21" s="71"/>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3100,6 +3123,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="M5:N5"/>
@@ -3108,14 +3139,6 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3123,10 +3146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E39BB3-9DB3-854C-B334-0F663BB94C97}">
-  <dimension ref="A1:S136"/>
+  <dimension ref="A1:T136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3137,12 +3160,12 @@
     <col min="17" max="17" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1" s="2">
         <v>44739</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -3151,26 +3174,26 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="62" t="s">
+      <c r="I5" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
       <c r="L5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="63"/>
+      <c r="N5" s="69"/>
       <c r="O5" s="18" t="s">
         <v>85</v>
       </c>
@@ -3181,115 +3204,115 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B6" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="64" t="s">
-        <v>149</v>
-      </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
+      <c r="I6" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
       <c r="L6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
       <c r="O6" s="17" t="s">
         <v>0</v>
       </c>
       <c r="P6" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q6" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="Q6" s="17" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="66"/>
-      <c r="K7" s="72"/>
+      <c r="I7" s="73" t="s">
+        <v>183</v>
+      </c>
+      <c r="J7" s="70"/>
+      <c r="K7" s="77"/>
       <c r="L7" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="65" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" s="72"/>
+      <c r="M7" s="73" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" s="77"/>
       <c r="O7" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="54" t="s">
-        <v>69</v>
+        <v>81</v>
+      </c>
+      <c r="P7" s="61" t="s">
+        <v>185</v>
       </c>
       <c r="Q7" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="60"/>
-      <c r="K8" s="69"/>
+      <c r="I8" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
       <c r="L8" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="M8" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="N8" s="60"/>
+      <c r="M8" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="81"/>
       <c r="O8" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="P8" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q8" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="P8" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q8" s="79" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B9" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
+      <c r="I9" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
       <c r="L9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="M9" s="66" t="s">
+      <c r="M9" s="70" t="s">
         <v>121</v>
       </c>
-      <c r="N9" s="66"/>
+      <c r="N9" s="70"/>
       <c r="O9" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P9" s="54">
         <v>65906</v>
@@ -3298,25 +3321,25 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="70" t="s">
+      <c r="I10" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
       <c r="L10" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="71" t="s">
+      <c r="M10" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="N10" s="71"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="55" t="s">
         <v>83</v>
       </c>
@@ -3326,7 +3349,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
         <v>25</v>
@@ -3335,7 +3358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="M14" s="57"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
@@ -3344,7 +3367,7 @@
       <c r="R14" s="16"/>
       <c r="S14" s="16"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -3355,7 +3378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>11</v>
       </c>
@@ -3387,14 +3410,12 @@
     <row r="21" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="C21" s="1"/>
-      <c r="E21" s="60" t="s">
+      <c r="E21" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="61"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3459,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
@@ -3659,7 +3680,7 @@
         <v>0</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -3681,7 +3702,7 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -3697,7 +3718,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -3797,7 +3818,7 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -3805,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="B67" s="58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -3839,7 +3860,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C77" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D77">
         <v>2000</v>
@@ -3850,7 +3871,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C79" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D79" s="8">
         <f>D81/D77</f>
@@ -3861,8 +3882,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C80" s="74" t="s">
-        <v>175</v>
+      <c r="C80" s="63" t="s">
+        <v>174</v>
       </c>
       <c r="D80" s="8">
         <f>D81</f>
@@ -3907,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="B88" s="58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -3920,7 +3941,7 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -3949,8 +3970,8 @@
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C98" s="74" t="s">
-        <v>175</v>
+      <c r="C98" s="63" t="s">
+        <v>174</v>
       </c>
       <c r="D98" s="8">
         <f>D99</f>
@@ -3982,7 +4003,7 @@
         <v>0</v>
       </c>
       <c r="B101" s="58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -3995,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="B105" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
@@ -4005,7 +4026,7 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C108" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D108">
         <v>500</v>
@@ -4013,10 +4034,10 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>181</v>
-      </c>
-      <c r="C109" s="75" t="s">
-        <v>176</v>
+        <v>180</v>
+      </c>
+      <c r="C109" s="64" t="s">
+        <v>175</v>
       </c>
       <c r="D109">
         <v>100</v>
@@ -4024,7 +4045,7 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C111" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D111" s="8">
         <f>D114/D108</f>
@@ -4035,8 +4056,8 @@
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C112" s="73" t="s">
-        <v>176</v>
+      <c r="C112" s="62" t="s">
+        <v>175</v>
       </c>
       <c r="D112" s="8">
         <f>D114/D109</f>
@@ -4047,8 +4068,8 @@
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C113" s="74" t="s">
-        <v>175</v>
+      <c r="C113" s="63" t="s">
+        <v>174</v>
       </c>
       <c r="D113" s="8">
         <f>D114</f>
@@ -4080,7 +4101,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
@@ -4096,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="B120" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
@@ -4156,7 +4177,7 @@
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C128" s="73" t="s">
+      <c r="C128" s="62" t="s">
         <v>37</v>
       </c>
       <c r="D128" s="8">
@@ -4187,7 +4208,7 @@
         <v>0</v>
       </c>
       <c r="B131" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.2">
@@ -4200,7 +4221,7 @@
         <v>0</v>
       </c>
       <c r="B133" s="58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10"/>
@@ -4236,20 +4257,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="M9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4259,8 +4280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B418F536-D2A8-4F42-BEB3-EBF867EDFB00}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4565,7 +4586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AA6687-62E1-8441-9354-0B15050C478B}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -4671,13 +4692,13 @@
         <v>134</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="K16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -4685,10 +4706,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -4748,7 +4769,7 @@
         <v>140</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -4768,7 +4789,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -4787,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -4803,7 +4824,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -4811,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -4832,7 +4853,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -4840,7 +4861,7 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>